<commit_message>
Sort Map by Value
</commit_message>
<xml_diff>
--- a/Files/Book1.xlsx
+++ b/Files/Book1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ytratsiuk/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ytratsiuk/IdeaProjects/TestProject/Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3B6D602B-AA00-D349-8EC0-F52FCC4BC639}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69B6E199-F296-9D4D-B408-B469290E9171}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3540" yWindow="820" windowWidth="26700" windowHeight="17320" xr2:uid="{EA2C8947-BEE1-4543-BBEF-D8F07C48099B}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17380" xr2:uid="{EA2C8947-BEE1-4543-BBEF-D8F07C48099B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>name</t>
   </si>
@@ -48,6 +48,24 @@
   </si>
   <si>
     <t>salary</t>
+  </si>
+  <si>
+    <t>marcel1</t>
+  </si>
+  <si>
+    <t>rodriguez</t>
+  </si>
+  <si>
+    <t>marcel2</t>
+  </si>
+  <si>
+    <t>marcel3</t>
+  </si>
+  <si>
+    <t>papaya</t>
+  </si>
+  <si>
+    <t>kiwi</t>
   </si>
 </sst>
 </file>
@@ -83,8 +101,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -399,32 +418,68 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C9F26BB-3DE8-AA48-87A5-A9B1633C2ABB}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
+      <c r="B3">
+        <v>39</v>
+      </c>
+      <c r="C3">
+        <v>32</v>
+      </c>
+      <c r="D3">
+        <v>12</v>
+      </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>340009</v>
+      </c>
+      <c r="C4">
+        <v>34000</v>
+      </c>
+      <c r="D4">
+        <v>10000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Storing Map in the List
</commit_message>
<xml_diff>
--- a/Files/Book1.xlsx
+++ b/Files/Book1.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ytratsiuk/IdeaProjects/TestProject/Files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pern-my.sharepoint.com/personal/shumaila_2838742_talmeez_pk/Documents/IntellijProjects/SDETJavaBatch15/Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69B6E199-F296-9D4D-B408-B469290E9171}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{82732E2D-864C-F944-97E4-4B647BCDD862}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6ACDA579-C28A-1E4C-B307-4E4DFAB6BF14}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17380" xr2:uid="{EA2C8947-BEE1-4543-BBEF-D8F07C48099B}"/>
+    <workbookView xWindow="54280" yWindow="500" windowWidth="14360" windowHeight="23500" activeTab="1" xr2:uid="{658EDF4E-4183-254E-A661-6B52BEB38FF1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,46 +37,78 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>last name</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+  <si>
+    <t>Name</t>
   </si>
   <si>
     <t>age</t>
   </si>
   <si>
+    <t>City</t>
+  </si>
+  <si>
     <t>salary</t>
   </si>
   <si>
-    <t>marcel1</t>
-  </si>
-  <si>
-    <t>rodriguez</t>
-  </si>
-  <si>
-    <t>marcel2</t>
-  </si>
-  <si>
-    <t>marcel3</t>
-  </si>
-  <si>
-    <t>papaya</t>
-  </si>
-  <si>
-    <t>kiwi</t>
+    <t>Hamid</t>
+  </si>
+  <si>
+    <t>San Ramon</t>
+  </si>
+  <si>
+    <t>Sam</t>
+  </si>
+  <si>
+    <t>Houston</t>
+  </si>
+  <si>
+    <t>Fayed</t>
+  </si>
+  <si>
+    <t>Alexandria</t>
+  </si>
+  <si>
+    <t>Useraname</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>asghar@gmail.com</t>
+  </si>
+  <si>
+    <t>123SKBDSSD+_#_$</t>
+  </si>
+  <si>
+    <t>asghar@gmail</t>
+  </si>
+  <si>
+    <t>asghar@gmail.</t>
+  </si>
+  <si>
+    <t>asghargmail.com</t>
+  </si>
+  <si>
+    <t>123SKBDSSD</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -98,14 +131,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -417,11 +452,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C9F26BB-3DE8-AA48-87A5-A9B1633C2ABB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A57E5B38-4223-E648-8B15-A22161041580}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView zoomScale="181" workbookViewId="0">
+      <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -431,58 +466,141 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>30</v>
+      </c>
+      <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
+      <c r="D2">
+        <v>120000</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B3">
-        <v>39</v>
-      </c>
-      <c r="C3">
-        <v>32</v>
+        <v>60</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
       </c>
       <c r="D3">
-        <v>12</v>
+        <v>125000</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1">
-        <v>340009</v>
-      </c>
-      <c r="C4">
-        <v>34000</v>
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>45</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
       </c>
       <c r="D4">
-        <v>10000</v>
+        <v>129000</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE666907-1196-604B-B849-6A0D146FEC3E}">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="132" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{EC243601-C879-2843-872C-2411CC5D222F}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{03AF00BE-DBC3-4442-9548-3483FA1B8F86}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{C0DB5080-0375-114A-8248-BF4D7A87DA83}"/>
+    <hyperlink ref="A5" r:id="rId4" display="asghar@gmail." xr:uid="{8A93B3AA-19F3-F848-9AE7-39F003EC0C68}"/>
+    <hyperlink ref="A6" r:id="rId5" display="asghar@gmail." xr:uid="{5A08D285-48C0-1543-A4BF-8278B5D47CEF}"/>
+    <hyperlink ref="A7" r:id="rId6" display="asghar@gmail." xr:uid="{CAF35A8A-26F7-3B46-9253-10CD56495F48}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>